<commit_message>
more call of cthulhu
</commit_message>
<xml_diff>
--- a/call-of-cthulhu-kadokawa/checklist.xlsx
+++ b/call-of-cthulhu-kadokawa/checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/call-of-cthulhu-kadokawa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{718A014C-A6AF-D14F-9C41-9153D7636C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5F4475-9DA8-0F4B-ACA7-296706C5F533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="460" windowWidth="26740" windowHeight="15780" xr2:uid="{81759EC4-D7E7-8642-A464-F1F22DE13120}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
   <si>
     <t>year</t>
   </si>
@@ -127,6 +127,63 @@
   </si>
   <si>
     <t>intro_to_cthulhu.jpg</t>
+  </si>
+  <si>
+    <t>d20_rulebook.jpg</t>
+  </si>
+  <si>
+    <t>コール オブ クトゥルフ d20</t>
+  </si>
+  <si>
+    <t>Call of Cthulhu d20</t>
+  </si>
+  <si>
+    <t>arkham.jpg</t>
+  </si>
+  <si>
+    <t>H.P.ラヴクラフト アーカム</t>
+  </si>
+  <si>
+    <t>H.P. Lovecraft's Arkham</t>
+  </si>
+  <si>
+    <t>クトゥルフ・ダークエイジ</t>
+  </si>
+  <si>
+    <t>Cthulhu Dark Ages</t>
+  </si>
+  <si>
+    <t>dark_ages.jpg</t>
+  </si>
+  <si>
+    <t>クトゥルフ神話TRPG 比叡山炎上</t>
+  </si>
+  <si>
+    <t>hieizan_flame.jpg</t>
+  </si>
+  <si>
+    <t>Hieizan Flame</t>
+  </si>
+  <si>
+    <t>seven_phantom_stories.jpg</t>
+  </si>
+  <si>
+    <t>scenario</t>
+  </si>
+  <si>
+    <t>Seven Phantom Stories</t>
+  </si>
+  <si>
+    <t>クトゥルフ神話TRPGシナリオ集 七つの怪談</t>
+  </si>
+  <si>
+    <t>クトゥルフ神話TRPG マレウス・モンストロルム</t>
+  </si>
+  <si>
+    <t>Malleus Monstrorum</t>
+  </si>
+  <si>
+    <t>malleus_monstrorum.jpg</t>
   </si>
 </sst>
 </file>
@@ -478,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2714E191-E70D-984A-B485-A0578E9C9933}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -651,6 +708,126 @@
         <v>16</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2003</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2004</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2005</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2006</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2007</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2008</v>
+      </c>
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>